<commit_message>
fix cancel act N0203-4
</commit_message>
<xml_diff>
--- a/Program/condition.xlsx
+++ b/Program/condition.xlsx
@@ -1,22 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion rupBuild="9303" lowestEdited="5" lastEdited="5" appName="xl"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="24332"/>
   <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_filtering\Program\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EB623C-FC10-4623-9A30-FA7484880527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="480" yWindow="60" windowWidth="18195" windowHeight="8505" activeTab="0"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet r:id="rId1" sheetId="1" name="เงื่อนไข"/>
-    <sheet r:id="rId2" sheetId="2" name="รหัสกิจกรรมยกเลิก"/>
-    <sheet r:id="rId3" sheetId="3" name="รหัส Product ยกเลิก"/>
+    <sheet name="เงื่อนไข" sheetId="1" r:id="rId1"/>
+    <sheet name="รหัสกิจกรรมยกเลิก" sheetId="2" r:id="rId2"/>
+    <sheet name="รหัส Product ยกเลิก" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr fullCalcOnLoad="1"/>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="598" uniqueCount="396">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="586" uniqueCount="396">
   <si>
     <t>รหัส</t>
   </si>
@@ -1032,18 +1038,12 @@
     <t>บันทึกรหัสกระบวนการทางธุรกิจ (กิจกรรม R, N, E)</t>
   </si>
   <si>
-    <t>[RNE].{0,4}$</t>
-  </si>
-  <si>
     <t>536017XX</t>
   </si>
   <si>
     <t>บันทึกรหัสกระบวนการทางธุรกิจ (N)</t>
   </si>
   <si>
-    <t>[N].{0,4}$</t>
-  </si>
-  <si>
     <t>546017XX</t>
   </si>
   <si>
@@ -1056,9 +1056,6 @@
     <t>บันทึกรหัสกระบวนการทางธุรกิจ</t>
   </si>
   <si>
-    <t>^.+$</t>
-  </si>
-  <si>
     <t>5X603XXX</t>
   </si>
   <si>
@@ -1131,89 +1128,95 @@
     <t>ยกเลิก/ห้ามบันทึก N0203</t>
   </si>
   <si>
+    <t>ยกเลิก/ห้ามบันทึก N0204</t>
+  </si>
+  <si>
+    <t>5X106XXX</t>
+  </si>
+  <si>
+    <t>ค่าอุปกรณ์และสายเคเบิล</t>
+  </si>
+  <si>
+    <t>5X643104</t>
+  </si>
+  <si>
+    <t>วัสดุทั่วไปใช้ไป</t>
+  </si>
+  <si>
+    <t>5X643106</t>
+  </si>
+  <si>
+    <t>ต-วัสดุแบบพิมพ์ใช้ไป</t>
+  </si>
+  <si>
+    <t>5X643206</t>
+  </si>
+  <si>
+    <t>ต-วัสดุแบบพิมพ์-จัดหาเอง</t>
+  </si>
+  <si>
+    <t>5X661XXX</t>
+  </si>
+  <si>
+    <t>ค่าสาธารณูปโภค</t>
+  </si>
+  <si>
+    <t>5X642108</t>
+  </si>
+  <si>
+    <t>ต-ค่าซ่อมแซมและบำรุงรักษา-ยานพาหนะ</t>
+  </si>
+  <si>
+    <t>บันทึกรหัสกระบวนการทางธุรกิจ (กิจกรรม E, N)</t>
+  </si>
+  <si>
+    <t>5X642112</t>
+  </si>
+  <si>
+    <t>ต-ค่าซ่อมแซมและบำรุงรักษา-ระบบเครื่องปรับอากาศ</t>
+  </si>
+  <si>
+    <t>บันทึกรหัสกระบวนการทางธุรกิจ (กิจกรรม E, J)</t>
+  </si>
+  <si>
+    <t>5XXXXXXX</t>
+  </si>
+  <si>
+    <t>ห้ามบันทึกรหัส Product ยกเลิก</t>
+  </si>
+  <si>
+    <t>cancel_product</t>
+  </si>
+  <si>
+    <t>ห้ามบันทึกรหัสกิจกรรมที่ยกเลิก</t>
+  </si>
+  <si>
+    <t>cancel_act</t>
+  </si>
+  <si>
     <t>N0203$</t>
   </si>
   <si>
-    <t>ยกเลิก/ห้ามบันทึก N0204</t>
+    <t>^(?!.*[RNE].{0,4}$)</t>
   </si>
   <si>
     <t>N0204$</t>
   </si>
   <si>
-    <t>5X106XXX</t>
-  </si>
-  <si>
-    <t>ค่าอุปกรณ์และสายเคเบิล</t>
-  </si>
-  <si>
-    <t>5X643104</t>
-  </si>
-  <si>
-    <t>วัสดุทั่วไปใช้ไป</t>
-  </si>
-  <si>
-    <t>5X643106</t>
-  </si>
-  <si>
-    <t>ต-วัสดุแบบพิมพ์ใช้ไป</t>
-  </si>
-  <si>
-    <t>5X643206</t>
-  </si>
-  <si>
-    <t>ต-วัสดุแบบพิมพ์-จัดหาเอง</t>
-  </si>
-  <si>
-    <t>5X661XXX</t>
-  </si>
-  <si>
-    <t>ค่าสาธารณูปโภค</t>
-  </si>
-  <si>
-    <t>5X642108</t>
-  </si>
-  <si>
-    <t>ต-ค่าซ่อมแซมและบำรุงรักษา-ยานพาหนะ</t>
-  </si>
-  <si>
-    <t>บันทึกรหัสกระบวนการทางธุรกิจ (กิจกรรม E, N)</t>
-  </si>
-  <si>
-    <t>[EJ].{0,4}$</t>
-  </si>
-  <si>
-    <t>5X642112</t>
-  </si>
-  <si>
-    <t>ต-ค่าซ่อมแซมและบำรุงรักษา-ระบบเครื่องปรับอากาศ</t>
-  </si>
-  <si>
-    <t>บันทึกรหัสกระบวนการทางธุรกิจ (กิจกรรม E, J)</t>
-  </si>
-  <si>
-    <t>5XXXXXXX</t>
-  </si>
-  <si>
-    <t>ห้ามบันทึกรหัส Product ยกเลิก</t>
-  </si>
-  <si>
-    <t>cancel_product</t>
-  </si>
-  <si>
-    <t>ห้ามบันทึกรหัสกิจกรรมที่ยกเลิก</t>
-  </si>
-  <si>
-    <t>cancel_act</t>
+    <t>^(?!.*[N].{0,4}$)</t>
+  </si>
+  <si>
+    <t>^(?!.*[EJ].{0,4}$)</t>
+  </si>
+  <si>
+    <t>^(?!.*[EN].{0,4}$)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="0.00e+00"/>
-  </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="4">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1282,83 +1285,89 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+  <cellXfs count="26">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="164" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
-    </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="3" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="2" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="3" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle xfId="0" builtinId="0" name="Normal"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
-    <ext uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14ac:slicerStyles xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" defaultSlicerStyle="SlicerStyleLight1"/>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -1369,10 +1378,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -1410,71 +1419,71 @@
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Times New Roman" script="Arab"/>
-        <a:font typeface="Times New Roman" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="MoolBoran" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Times New Roman" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
-        <a:font typeface="ＭＳ Ｐゴシック" script="Jpan"/>
-        <a:font typeface="맑은 고딕" script="Hang"/>
-        <a:font typeface="宋体" script="Hans"/>
-        <a:font typeface="新細明體" script="Hant"/>
-        <a:font typeface="Arial" script="Arab"/>
-        <a:font typeface="Arial" script="Hebr"/>
-        <a:font typeface="Tahoma" script="Thai"/>
-        <a:font typeface="Nyala" script="Ethi"/>
-        <a:font typeface="Vrinda" script="Beng"/>
-        <a:font typeface="Shruti" script="Gujr"/>
-        <a:font typeface="DaunPenh" script="Khmr"/>
-        <a:font typeface="Tunga" script="Knda"/>
-        <a:font typeface="Raavi" script="Guru"/>
-        <a:font typeface="Euphemia" script="Cans"/>
-        <a:font typeface="Plantagenet Cherokee" script="Cher"/>
-        <a:font typeface="Microsoft Yi Baiti" script="Yiii"/>
-        <a:font typeface="Microsoft Himalaya" script="Tibt"/>
-        <a:font typeface="MV Boli" script="Thaa"/>
-        <a:font typeface="Mangal" script="Deva"/>
-        <a:font typeface="Gautami" script="Telu"/>
-        <a:font typeface="Latha" script="Taml"/>
-        <a:font typeface="Estrangelo Edessa" script="Syrc"/>
-        <a:font typeface="Kalinga" script="Orya"/>
-        <a:font typeface="Kartika" script="Mlym"/>
-        <a:font typeface="DokChampa" script="Laoo"/>
-        <a:font typeface="Iskoola Pota" script="Sinh"/>
-        <a:font typeface="Mongolian Baiti" script="Mong"/>
-        <a:font typeface="Arial" script="Viet"/>
-        <a:font typeface="Microsoft Uighur" script="Uigh"/>
-        <a:font typeface="Sylfaen" script="Geor"/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1502,7 +1511,7 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
         <a:gradFill rotWithShape="1">
           <a:gsLst>
@@ -1525,11 +1534,11 @@
               </a:schemeClr>
             </a:gs>
           </a:gsLst>
-          <a:lin scaled="1" ang="16200000"/>
+          <a:lin ang="16200000" scaled="1"/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="9525">
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr">
               <a:shade val="9500"/>
@@ -1538,13 +1547,13 @@
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
         </a:ln>
-        <a:ln algn="ctr" cmpd="sng" cap="flat" w="38100">
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -1554,7 +1563,7 @@
       <a:effectStyleLst>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="38000"/>
               </a:srgbClr>
@@ -1563,7 +1572,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1572,7 +1581,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw dir="5400000" rotWithShape="0" dist="23000" blurRad="40000">
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="35000"/>
               </a:srgbClr>
@@ -1580,10 +1589,10 @@
           </a:effectLst>
           <a:scene3d>
             <a:camera prst="orthographicFront">
-              <a:rot rev="0" lon="0" lat="0"/>
+              <a:rot lat="0" lon="0" rev="0"/>
             </a:camera>
-            <a:lightRig dir="t" rig="threePt">
-              <a:rot rev="1200000" lon="0" lat="0"/>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
             </a:lightRig>
           </a:scene3d>
           <a:sp3d>
@@ -1648,25 +1657,27 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
-  <dimension ref="A1:F25"/>
+  <dimension ref="A1:F24"/>
   <sheetViews>
-    <sheetView workbookViewId="0" tabSelected="1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F16" sqref="F16"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="21" width="22.005" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="22" width="49.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="22" width="43.86214285714286" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="22" width="38.43357142857143" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="19.005" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="22.433571428571426" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="22" style="21" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="49.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="43.85546875" style="22" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="38.42578125" style="22" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.5703125" style="5" customWidth="1"/>
+    <col min="6" max="6" width="22.42578125" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75" customFormat="1" s="12">
+    <row r="1" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
@@ -1686,7 +1697,7 @@
         <v>334</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75" customFormat="1" s="12">
+    <row r="2" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A2" s="13" t="s">
         <v>335</v>
       </c>
@@ -1698,369 +1709,335 @@
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15" t="s">
+        <v>391</v>
+      </c>
+      <c r="F2" s="15"/>
+    </row>
+    <row r="3" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A3" s="13" t="s">
         <v>338</v>
-      </c>
-      <c r="F2" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A3" s="13" t="s">
-        <v>339</v>
       </c>
       <c r="B3" s="14" t="s">
         <v>336</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15" t="s">
-        <v>341</v>
+        <v>393</v>
       </c>
       <c r="F3" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75" customFormat="1" s="12">
+    <row r="4" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A4" s="13" t="s">
-        <v>342</v>
+        <v>340</v>
       </c>
       <c r="B4" s="14" t="s">
         <v>336</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15" t="s">
+        <v>393</v>
+      </c>
+      <c r="F4" s="15"/>
+    </row>
+    <row r="5" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A5" s="13" t="s">
         <v>341</v>
       </c>
-      <c r="F4" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A5" s="13" t="s">
+      <c r="B5" s="14" t="s">
+        <v>342</v>
+      </c>
+      <c r="C5" s="14" t="s">
         <v>343</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
+    </row>
+    <row r="6" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A6" s="13" t="s">
         <v>344</v>
       </c>
-      <c r="C5" s="14" t="s">
+      <c r="B6" s="14" t="s">
         <v>345</v>
       </c>
-      <c r="D5" s="15"/>
-      <c r="E5" s="15" t="s">
+      <c r="C6" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
+    </row>
+    <row r="7" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A7" s="13" t="s">
         <v>346</v>
       </c>
-      <c r="F5" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A6" s="13" t="s">
+      <c r="B7" s="14" t="s">
         <v>347</v>
       </c>
-      <c r="B6" s="14" t="s">
+      <c r="C7" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D7" s="15"/>
+      <c r="E7" s="15"/>
+      <c r="F7" s="15"/>
+    </row>
+    <row r="8" spans="1:6" ht="18.75" customHeight="1">
+      <c r="A8" s="13" t="s">
         <v>348</v>
       </c>
-      <c r="C6" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D6" s="15"/>
-      <c r="E6" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="F6" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A7" s="13" t="s">
+      <c r="B8" s="14" t="s">
         <v>349</v>
       </c>
-      <c r="B7" s="14" t="s">
+      <c r="C8" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D8" s="15" t="s">
         <v>350</v>
       </c>
-      <c r="C7" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D7" s="15"/>
-      <c r="E7" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="F7" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="13" t="s">
+      <c r="E8" s="2"/>
+      <c r="F8" s="16" t="s">
         <v>351</v>
       </c>
-      <c r="B8" s="14" t="s">
+    </row>
+    <row r="9" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A9" s="13" t="s">
         <v>352</v>
-      </c>
-      <c r="C8" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D8" s="15" t="s">
-        <v>353</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>346</v>
-      </c>
-      <c r="F8" s="16" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A9" s="13" t="s">
-        <v>355</v>
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>356</v>
+        <v>353</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15" t="s">
-        <v>357</v>
+        <v>354</v>
       </c>
       <c r="F9" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75" customFormat="1" s="12">
+    <row r="10" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
-        <v>359</v>
+        <v>356</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15" t="s">
-        <v>360</v>
+        <v>357</v>
       </c>
       <c r="F10" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75" customFormat="1" s="12">
+    <row r="11" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>358</v>
+        <v>355</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14" t="s">
-        <v>361</v>
+        <v>358</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15" t="s">
+        <v>359</v>
+      </c>
+      <c r="F11" s="15"/>
+    </row>
+    <row r="12" spans="1:6" s="12" customFormat="1" ht="21" customHeight="1">
+      <c r="A12" s="17" t="s">
+        <v>360</v>
+      </c>
+      <c r="B12" s="18" t="s">
+        <v>361</v>
+      </c>
+      <c r="C12" s="14" t="s">
         <v>362</v>
-      </c>
-      <c r="F11" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="21" customFormat="1" s="12">
-      <c r="A12" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="B12" s="18" t="s">
-        <v>364</v>
-      </c>
-      <c r="C12" s="14" t="s">
-        <v>365</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
+        <v>363</v>
+      </c>
+      <c r="F12" s="14"/>
+    </row>
+    <row r="13" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A13" s="13" t="s">
+        <v>364</v>
+      </c>
+      <c r="B13" s="14" t="s">
+        <v>365</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D13" s="15"/>
+      <c r="E13" s="15"/>
+      <c r="F13" s="15"/>
+    </row>
+    <row r="14" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A14" s="13" t="s">
         <v>366</v>
-      </c>
-      <c r="F12" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A13" s="13" t="s">
-        <v>367</v>
-      </c>
-      <c r="B13" s="14" t="s">
-        <v>368</v>
-      </c>
-      <c r="C13" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D13" s="15"/>
-      <c r="E13" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="F13" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A14" s="13" t="s">
-        <v>369</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14" t="s">
-        <v>370</v>
+        <v>367</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15" t="s">
-        <v>371</v>
+        <v>390</v>
       </c>
       <c r="F14" s="15"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75" customFormat="1" s="12">
+    <row r="15" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A15" s="13" t="s">
-        <v>369</v>
+        <v>366</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15" t="s">
+        <v>392</v>
+      </c>
+      <c r="F15" s="15"/>
+    </row>
+    <row r="16" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A16" s="13" t="s">
+        <v>369</v>
+      </c>
+      <c r="B16" s="14" t="s">
+        <v>370</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D16" s="15"/>
+      <c r="E16" s="15"/>
+      <c r="F16" s="15"/>
+    </row>
+    <row r="17" spans="1:6" s="12" customFormat="1" ht="19.5" customHeight="1">
+      <c r="A17" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B17" s="14" t="s">
+        <v>372</v>
+      </c>
+      <c r="C17" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D17" s="14"/>
+      <c r="E17" s="14"/>
+      <c r="F17" s="14"/>
+    </row>
+    <row r="18" spans="1:6" s="12" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A18" s="17" t="s">
         <v>373</v>
       </c>
-      <c r="F15" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A16" s="13" t="s">
+      <c r="B18" s="18" t="s">
         <v>374</v>
       </c>
-      <c r="B16" s="14" t="s">
+      <c r="C18" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D18" s="14"/>
+      <c r="E18" s="14"/>
+      <c r="F18" s="14"/>
+    </row>
+    <row r="19" spans="1:6" s="12" customFormat="1" ht="21" customHeight="1">
+      <c r="A19" s="17" t="s">
         <v>375</v>
       </c>
-      <c r="C16" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D16" s="15"/>
-      <c r="E16" s="15" t="s">
-        <v>346</v>
-      </c>
-      <c r="F16" s="15"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="19.5" customFormat="1" s="12">
-      <c r="A17" s="17" t="s">
+      <c r="B19" s="18" t="s">
         <v>376</v>
       </c>
-      <c r="B17" s="14" t="s">
+      <c r="C19" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D19" s="14"/>
+      <c r="E19" s="14"/>
+      <c r="F19" s="14"/>
+    </row>
+    <row r="20" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
+      <c r="A20" s="19" t="s">
         <v>377</v>
       </c>
-      <c r="C17" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D17" s="14"/>
-      <c r="E17" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="F17" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="20.25" customFormat="1" s="12">
-      <c r="A18" s="17" t="s">
+      <c r="B20" s="14" t="s">
         <v>378</v>
       </c>
-      <c r="B18" s="18" t="s">
+      <c r="C20" s="14" t="s">
+        <v>343</v>
+      </c>
+      <c r="D20" s="14"/>
+      <c r="E20" s="14"/>
+      <c r="F20" s="14"/>
+    </row>
+    <row r="21" spans="1:6" s="12" customFormat="1" ht="20.25" customHeight="1">
+      <c r="A21" s="17" t="s">
         <v>379</v>
       </c>
-      <c r="C18" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="F18" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="21" customFormat="1" s="12">
-      <c r="A19" s="17" t="s">
+      <c r="B21" s="18" t="s">
         <v>380</v>
       </c>
-      <c r="B19" s="18" t="s">
+      <c r="C21" s="14" t="s">
         <v>381</v>
-      </c>
-      <c r="C19" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D19" s="14"/>
-      <c r="E19" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="F19" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A20" s="19" t="s">
-        <v>382</v>
-      </c>
-      <c r="B20" s="14" t="s">
-        <v>383</v>
-      </c>
-      <c r="C20" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D20" s="14"/>
-      <c r="E20" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="F20" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="20.25" customFormat="1" s="12">
-      <c r="A21" s="17" t="s">
-        <v>384</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>385</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>386</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14" t="s">
-        <v>387</v>
+        <v>395</v>
       </c>
       <c r="F21" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="20.25" customFormat="1" s="12">
+    <row r="22" spans="1:6" s="12" customFormat="1" ht="20.25" customHeight="1">
       <c r="A22" s="17" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14" t="s">
-        <v>387</v>
+        <v>394</v>
       </c>
       <c r="F22" s="14"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:6" ht="18.75" customHeight="1">
       <c r="A23" s="17" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="9" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="F23" s="2"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75" customFormat="1" s="12">
+    <row r="24" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A24" s="17" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>364</v>
+        <v>361</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="F24" s="14"/>
-    </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75" customFormat="1" s="12">
-      <c r="A25" s="17">
-        <v>53601709</v>
-      </c>
-      <c r="B25" s="14"/>
-      <c r="C25" s="14" t="s">
-        <v>345</v>
-      </c>
-      <c r="D25" s="14"/>
-      <c r="E25" s="14" t="s">
-        <v>346</v>
-      </c>
-      <c r="F25" s="14"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2068,7 +2045,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
@@ -2076,22 +2053,21 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="10" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="11" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="3" max="3" style="5" width="21.719285714285714" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="5" max="5" style="5" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="6" max="6" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="7" max="7" style="4" width="10.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="8" max="8" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="9" max="9" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="10" max="10" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="11" max="11" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="13.5703125" style="10" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.5703125" style="11" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.7109375" style="5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="4" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="13.5703125" style="5" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.5703125" style="4" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row r="1" spans="1:11" ht="18.75" customHeight="1">
       <c r="A1" s="6" t="s">
         <v>109</v>
       </c>
@@ -2122,7 +2098,7 @@
         <v>116</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
+    <row r="2" spans="1:11" ht="18.75" customHeight="1">
       <c r="A2" s="8" t="s">
         <v>117</v>
       </c>
@@ -2153,7 +2129,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
+    <row r="3" spans="1:11" ht="18.75" customHeight="1">
       <c r="A3" s="8" t="s">
         <v>123</v>
       </c>
@@ -2184,7 +2160,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
+    <row r="4" spans="1:11" ht="18.75" customHeight="1">
       <c r="A4" s="8" t="s">
         <v>126</v>
       </c>
@@ -2215,7 +2191,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
+    <row r="5" spans="1:11" ht="18.75" customHeight="1">
       <c r="A5" s="8" t="s">
         <v>129</v>
       </c>
@@ -2246,7 +2222,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
+    <row r="6" spans="1:11" ht="18.75" customHeight="1">
       <c r="A6" s="8" t="s">
         <v>132</v>
       </c>
@@ -2277,7 +2253,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
+    <row r="7" spans="1:11" ht="18.75" customHeight="1">
       <c r="A7" s="8" t="s">
         <v>135</v>
       </c>
@@ -2308,7 +2284,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
+    <row r="8" spans="1:11" ht="18.75" customHeight="1">
       <c r="A8" s="8" t="s">
         <v>138</v>
       </c>
@@ -2339,7 +2315,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
+    <row r="9" spans="1:11" ht="18.75" customHeight="1">
       <c r="A9" s="8" t="s">
         <v>141</v>
       </c>
@@ -2370,7 +2346,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
+    <row r="10" spans="1:11" ht="18.75" customHeight="1">
       <c r="A10" s="8" t="s">
         <v>144</v>
       </c>
@@ -2401,7 +2377,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
+    <row r="11" spans="1:11" ht="18.75" customHeight="1">
       <c r="A11" s="8" t="s">
         <v>147</v>
       </c>
@@ -2432,7 +2408,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
+    <row r="12" spans="1:11" ht="18.75" customHeight="1">
       <c r="A12" s="8" t="s">
         <v>150</v>
       </c>
@@ -2463,7 +2439,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
+    <row r="13" spans="1:11" ht="18.75" customHeight="1">
       <c r="A13" s="8" t="s">
         <v>153</v>
       </c>
@@ -2494,7 +2470,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
+    <row r="14" spans="1:11" ht="18.75" customHeight="1">
       <c r="A14" s="8" t="s">
         <v>156</v>
       </c>
@@ -2525,7 +2501,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
+    <row r="15" spans="1:11" ht="18.75" customHeight="1">
       <c r="A15" s="8" t="s">
         <v>159</v>
       </c>
@@ -2556,7 +2532,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
+    <row r="16" spans="1:11" ht="18.75" customHeight="1">
       <c r="A16" s="8" t="s">
         <v>162</v>
       </c>
@@ -2587,7 +2563,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
+    <row r="17" spans="1:11" ht="18.75" customHeight="1">
       <c r="A17" s="8" t="s">
         <v>165</v>
       </c>
@@ -2618,7 +2594,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
+    <row r="18" spans="1:11" ht="18.75" customHeight="1">
       <c r="A18" s="8" t="s">
         <v>168</v>
       </c>
@@ -2649,7 +2625,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
+    <row r="19" spans="1:11" ht="18.75" customHeight="1">
       <c r="A19" s="8" t="s">
         <v>171</v>
       </c>
@@ -2680,7 +2656,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
+    <row r="20" spans="1:11" ht="18.75" customHeight="1">
       <c r="A20" s="8" t="s">
         <v>174</v>
       </c>
@@ -2711,7 +2687,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
+    <row r="21" spans="1:11" ht="18.75" customHeight="1">
       <c r="A21" s="8" t="s">
         <v>177</v>
       </c>
@@ -2742,7 +2718,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
+    <row r="22" spans="1:11" ht="18.75" customHeight="1">
       <c r="A22" s="8" t="s">
         <v>180</v>
       </c>
@@ -2773,7 +2749,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
+    <row r="23" spans="1:11" ht="18.75" customHeight="1">
       <c r="A23" s="8" t="s">
         <v>183</v>
       </c>
@@ -2804,7 +2780,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
+    <row r="24" spans="1:11" ht="18.75" customHeight="1">
       <c r="A24" s="8" t="s">
         <v>186</v>
       </c>
@@ -2835,7 +2811,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
+    <row r="25" spans="1:11" ht="18.75" customHeight="1">
       <c r="A25" s="8" t="s">
         <v>189</v>
       </c>
@@ -2866,7 +2842,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
+    <row r="26" spans="1:11" ht="18.75" customHeight="1">
       <c r="A26" s="8" t="s">
         <v>192</v>
       </c>
@@ -2897,7 +2873,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
+    <row r="27" spans="1:11" ht="18.75" customHeight="1">
       <c r="A27" s="8" t="s">
         <v>195</v>
       </c>
@@ -2928,7 +2904,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
+    <row r="28" spans="1:11" ht="18.75" customHeight="1">
       <c r="A28" s="8" t="s">
         <v>198</v>
       </c>
@@ -2959,7 +2935,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
+    <row r="29" spans="1:11" ht="18.75" customHeight="1">
       <c r="A29" s="8" t="s">
         <v>201</v>
       </c>
@@ -2990,7 +2966,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
+    <row r="30" spans="1:11" ht="18.75" customHeight="1">
       <c r="A30" s="8" t="s">
         <v>204</v>
       </c>
@@ -3021,7 +2997,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
+    <row r="31" spans="1:11" ht="18.75" customHeight="1">
       <c r="A31" s="8" t="s">
         <v>207</v>
       </c>
@@ -3052,7 +3028,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
+    <row r="32" spans="1:11" ht="18.75" customHeight="1">
       <c r="A32" s="8" t="s">
         <v>210</v>
       </c>
@@ -3083,7 +3059,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
+    <row r="33" spans="1:11" ht="18.75" customHeight="1">
       <c r="A33" s="8" t="s">
         <v>213</v>
       </c>
@@ -3114,7 +3090,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
+    <row r="34" spans="1:11" ht="18.75" customHeight="1">
       <c r="A34" s="8" t="s">
         <v>216</v>
       </c>
@@ -3145,7 +3121,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
+    <row r="35" spans="1:11" ht="18.75" customHeight="1">
       <c r="A35" s="8" t="s">
         <v>219</v>
       </c>
@@ -3176,7 +3152,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
+    <row r="36" spans="1:11" ht="18.75" customHeight="1">
       <c r="A36" s="8" t="s">
         <v>222</v>
       </c>
@@ -3207,7 +3183,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
+    <row r="37" spans="1:11" ht="18.75" customHeight="1">
       <c r="A37" s="8" t="s">
         <v>225</v>
       </c>
@@ -3238,7 +3214,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row r="38" spans="1:11" ht="18.75" customHeight="1">
       <c r="A38" s="8" t="s">
         <v>228</v>
       </c>
@@ -3269,7 +3245,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row r="39" spans="1:11" ht="18.75" customHeight="1">
       <c r="A39" s="8" t="s">
         <v>231</v>
       </c>
@@ -3300,7 +3276,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row r="40" spans="1:11" ht="18.75" customHeight="1">
       <c r="A40" s="6" t="s">
         <v>234</v>
       </c>
@@ -3329,7 +3305,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row r="41" spans="1:11" ht="18.75" customHeight="1">
       <c r="A41" s="6" t="s">
         <v>238</v>
       </c>
@@ -3358,7 +3334,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
+    <row r="42" spans="1:11" ht="18.75" customHeight="1">
       <c r="A42" s="6" t="s">
         <v>242</v>
       </c>
@@ -3387,7 +3363,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
+    <row r="43" spans="1:11" ht="18.75" customHeight="1">
       <c r="A43" s="6" t="s">
         <v>245</v>
       </c>
@@ -3416,7 +3392,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
+    <row r="44" spans="1:11" ht="18.75" customHeight="1">
       <c r="A44" s="6" t="s">
         <v>249</v>
       </c>
@@ -3445,7 +3421,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
+    <row r="45" spans="1:11" ht="18.75" customHeight="1">
       <c r="A45" s="6" t="s">
         <v>252</v>
       </c>
@@ -3474,7 +3450,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
+    <row r="46" spans="1:11" ht="18.75" customHeight="1">
       <c r="A46" s="6" t="s">
         <v>255</v>
       </c>
@@ -3503,7 +3479,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
+    <row r="47" spans="1:11" ht="18.75" customHeight="1">
       <c r="A47" s="6" t="s">
         <v>258</v>
       </c>
@@ -3532,7 +3508,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
+    <row r="48" spans="1:11" ht="18.75" customHeight="1">
       <c r="A48" s="6" t="s">
         <v>261</v>
       </c>
@@ -3561,7 +3537,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
+    <row r="49" spans="1:11" ht="18.75" customHeight="1">
       <c r="A49" s="6" t="s">
         <v>264</v>
       </c>
@@ -3590,7 +3566,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
+    <row r="50" spans="1:11" ht="18.75" customHeight="1">
       <c r="A50" s="6" t="s">
         <v>267</v>
       </c>
@@ -3619,7 +3595,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
+    <row r="51" spans="1:11" ht="18.75" customHeight="1">
       <c r="A51" s="6" t="s">
         <v>271</v>
       </c>
@@ -3648,7 +3624,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
+    <row r="52" spans="1:11" ht="18.75" customHeight="1">
       <c r="A52" s="6" t="s">
         <v>274</v>
       </c>
@@ -3677,7 +3653,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
+    <row r="53" spans="1:11" ht="18.75" customHeight="1">
       <c r="A53" s="6" t="s">
         <v>277</v>
       </c>
@@ -3706,7 +3682,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
+    <row r="54" spans="1:11" ht="18.75" customHeight="1">
       <c r="A54" s="6" t="s">
         <v>280</v>
       </c>
@@ -3735,7 +3711,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
+    <row r="55" spans="1:11" ht="18.75" customHeight="1">
       <c r="A55" s="6" t="s">
         <v>283</v>
       </c>
@@ -3764,7 +3740,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
+    <row r="56" spans="1:11" ht="18.75" customHeight="1">
       <c r="A56" s="6" t="s">
         <v>286</v>
       </c>
@@ -3793,7 +3769,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
+    <row r="57" spans="1:11" ht="18.75" customHeight="1">
       <c r="A57" s="6" t="s">
         <v>289</v>
       </c>
@@ -3822,7 +3798,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
+    <row r="58" spans="1:11" ht="18.75" customHeight="1">
       <c r="A58" s="6" t="s">
         <v>292</v>
       </c>
@@ -3851,7 +3827,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
+    <row r="59" spans="1:11" ht="18.75" customHeight="1">
       <c r="A59" s="6" t="s">
         <v>295</v>
       </c>
@@ -3880,7 +3856,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
+    <row r="60" spans="1:11" ht="18.75" customHeight="1">
       <c r="A60" s="6" t="s">
         <v>298</v>
       </c>
@@ -3909,7 +3885,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
+    <row r="61" spans="1:11" ht="18.75" customHeight="1">
       <c r="A61" s="6" t="s">
         <v>301</v>
       </c>
@@ -3938,7 +3914,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
+    <row r="62" spans="1:11" ht="18.75" customHeight="1">
       <c r="A62" s="6" t="s">
         <v>304</v>
       </c>
@@ -3967,7 +3943,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
+    <row r="63" spans="1:11" ht="18.75" customHeight="1">
       <c r="A63" s="6" t="s">
         <v>307</v>
       </c>
@@ -3996,7 +3972,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
+    <row r="64" spans="1:11" ht="18.75" customHeight="1">
       <c r="A64" s="6" t="s">
         <v>310</v>
       </c>
@@ -4025,7 +4001,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
+    <row r="65" spans="1:11" ht="18.75" customHeight="1">
       <c r="A65" s="6" t="s">
         <v>313</v>
       </c>
@@ -4054,7 +4030,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
+    <row r="66" spans="1:11" ht="18.75" customHeight="1">
       <c r="A66" s="6" t="s">
         <v>316</v>
       </c>
@@ -4083,7 +4059,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
+    <row r="67" spans="1:11" ht="18.75" customHeight="1">
       <c r="A67" s="6" t="s">
         <v>319</v>
       </c>
@@ -4112,7 +4088,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
+    <row r="68" spans="1:11" ht="18.75" customHeight="1">
       <c r="A68" s="6" t="s">
         <v>322</v>
       </c>
@@ -4141,7 +4117,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
+    <row r="69" spans="1:11" ht="18.75" customHeight="1">
       <c r="A69" s="6" t="s">
         <v>325</v>
       </c>
@@ -4170,7 +4146,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
+    <row r="70" spans="1:11" ht="18.75" customHeight="1">
       <c r="A70" s="6" t="s">
         <v>328</v>
       </c>
@@ -4205,878 +4181,880 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0"/>
   </sheetPr>
   <dimension ref="A1:B108"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I11" sqref="I11"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" style="4" width="9.719285714285713" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="5" width="22.290714285714284" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" width="11.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.28515625" style="5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A1" s="23" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="18.75">
-      <c r="A2" s="3">
+    <row r="2" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A2" s="24">
         <v>101010001</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="18.75">
-      <c r="A3" s="3">
+    <row r="3" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A3" s="24">
         <v>101010002</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="18.75">
-      <c r="A4" s="3">
+    <row r="4" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A4" s="24">
         <v>101010004</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>4</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="18.75">
-      <c r="A5" s="3">
+    <row r="5" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A5" s="24">
         <v>101010006</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="18.75">
-      <c r="A6" s="3">
+    <row r="6" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A6" s="24">
         <v>101010009</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>6</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="18.75">
-      <c r="A7" s="3">
+    <row r="7" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A7" s="24">
         <v>101010010</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="18.75">
-      <c r="A8" s="3">
+    <row r="8" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A8" s="24">
         <v>101010012</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="3">
+    <row r="9" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A9" s="24">
         <v>101010013</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="3">
+    <row r="10" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A10" s="24">
         <v>101010015</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="11" customHeight="1" ht="18.75">
-      <c r="A11" s="3">
+    <row r="11" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A11" s="24">
         <v>101010016</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="12" customHeight="1" ht="18.75">
-      <c r="A12" s="3">
+    <row r="12" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A12" s="24">
         <v>101010019</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="13" customHeight="1" ht="18.75">
-      <c r="A13" s="3">
+    <row r="13" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A13" s="24">
         <v>101014100</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="14" customHeight="1" ht="18.75">
-      <c r="A14" s="3">
+    <row r="14" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A14" s="24">
         <v>101019901</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>14</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="15" customHeight="1" ht="18.75">
-      <c r="A15" s="3">
+    <row r="15" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A15" s="24">
         <v>102010102</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>15</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="16" customHeight="1" ht="18.75">
-      <c r="A16" s="3">
+    <row r="16" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A16" s="24">
         <v>102010103</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>16</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="17" customHeight="1" ht="18.75">
-      <c r="A17" s="3">
+    <row r="17" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A17" s="24">
         <v>102010202</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="18" customHeight="1" ht="18.75">
-      <c r="A18" s="3">
+    <row r="18" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A18" s="24">
         <v>102010205</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>18</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="19" customHeight="1" ht="18.75">
-      <c r="A19" s="3">
+    <row r="19" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A19" s="24">
         <v>102010207</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>19</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="20" customHeight="1" ht="18.75">
-      <c r="A20" s="3">
+    <row r="20" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A20" s="24">
         <v>102010301</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>20</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="21" customHeight="1" ht="18.75">
-      <c r="A21" s="3">
+    <row r="21" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A21" s="24">
         <v>102010302</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>21</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="22" customHeight="1" ht="18.75">
-      <c r="A22" s="3">
+    <row r="22" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A22" s="24">
         <v>102010408</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>22</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="23" customHeight="1" ht="18.75">
-      <c r="A23" s="3">
+    <row r="23" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A23" s="24">
         <v>102014100</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>23</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="24" customHeight="1" ht="18.75">
-      <c r="A24" s="3">
+    <row r="24" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A24" s="24">
         <v>102020006</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>24</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="25" customHeight="1" ht="18.75">
-      <c r="A25" s="3">
+    <row r="25" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A25" s="24">
         <v>102020008</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>25</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="26" customHeight="1" ht="18.75">
-      <c r="A26" s="3">
+    <row r="26" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A26" s="24">
         <v>102020016</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>26</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="27" customHeight="1" ht="18.75">
-      <c r="A27" s="3">
+    <row r="27" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A27" s="24">
         <v>102024100</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>27</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="28" customHeight="1" ht="18.75">
-      <c r="A28" s="3">
+    <row r="28" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A28" s="24">
         <v>102030010</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>28</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="29" customHeight="1" ht="18.75">
-      <c r="A29" s="3">
+    <row r="29" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A29" s="24">
         <v>102030018</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>29</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="30" customHeight="1" ht="18.75">
-      <c r="A30" s="3">
+    <row r="30" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A30" s="24">
         <v>102034100</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>30</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="31" customHeight="1" ht="18.75">
-      <c r="A31" s="3">
+    <row r="31" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A31" s="24">
         <v>102039901</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>31</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="32" customHeight="1" ht="18.75">
-      <c r="A32" s="3">
+    <row r="32" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A32" s="24">
         <v>103010002</v>
       </c>
       <c r="B32" s="2" t="s">
         <v>32</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="33" customHeight="1" ht="18.75">
-      <c r="A33" s="3">
+    <row r="33" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A33" s="24">
         <v>103010005</v>
       </c>
       <c r="B33" s="2" t="s">
         <v>33</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="34" customHeight="1" ht="18.75">
-      <c r="A34" s="3">
+    <row r="34" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A34" s="24">
         <v>103010006</v>
       </c>
       <c r="B34" s="2" t="s">
         <v>34</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="35" customHeight="1" ht="18.75">
-      <c r="A35" s="3">
+    <row r="35" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A35" s="24">
         <v>103010012</v>
       </c>
       <c r="B35" s="2" t="s">
         <v>35</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="36" customHeight="1" ht="18.75">
-      <c r="A36" s="3">
+    <row r="36" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A36" s="24">
         <v>103010013</v>
       </c>
       <c r="B36" s="2" t="s">
         <v>36</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="37" customHeight="1" ht="18.75">
-      <c r="A37" s="3">
+    <row r="37" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A37" s="24">
         <v>103010019</v>
       </c>
       <c r="B37" s="2" t="s">
         <v>37</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
-      <c r="A38" s="3">
+    <row r="38" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A38" s="24">
         <v>103010029</v>
       </c>
       <c r="B38" s="2" t="s">
         <v>38</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
-      <c r="A39" s="3">
+    <row r="39" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A39" s="24">
         <v>103010032</v>
       </c>
       <c r="B39" s="2" t="s">
         <v>39</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
-      <c r="A40" s="3">
+    <row r="40" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A40" s="24">
         <v>103010035</v>
       </c>
       <c r="B40" s="2" t="s">
         <v>40</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
-      <c r="A41" s="3">
+    <row r="41" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A41" s="24">
         <v>103010037</v>
       </c>
       <c r="B41" s="2" t="s">
         <v>41</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="42" customHeight="1" ht="18.75">
-      <c r="A42" s="3">
+    <row r="42" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A42" s="24">
         <v>103014100</v>
       </c>
       <c r="B42" s="2" t="s">
         <v>42</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="43" customHeight="1" ht="18.75">
-      <c r="A43" s="3">
+    <row r="43" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A43" s="24">
         <v>103019901</v>
       </c>
       <c r="B43" s="2" t="s">
         <v>43</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="44" customHeight="1" ht="18.75">
-      <c r="A44" s="3">
+    <row r="44" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A44" s="24">
         <v>103029901</v>
       </c>
       <c r="B44" s="2" t="s">
         <v>44</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="45" customHeight="1" ht="18.75">
-      <c r="A45" s="3">
+    <row r="45" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A45" s="24">
         <v>104010014</v>
       </c>
       <c r="B45" s="2" t="s">
         <v>45</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="46" customHeight="1" ht="18.75">
-      <c r="A46" s="3">
+    <row r="46" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A46" s="24">
         <v>104010015</v>
       </c>
       <c r="B46" s="2" t="s">
         <v>46</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="47" customHeight="1" ht="18.75">
-      <c r="A47" s="3">
+    <row r="47" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A47" s="24">
         <v>104010016</v>
       </c>
       <c r="B47" s="2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="48" customHeight="1" ht="18.75">
-      <c r="A48" s="3">
+    <row r="48" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A48" s="24">
         <v>104010017</v>
       </c>
       <c r="B48" s="2" t="s">
         <v>48</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="49" customHeight="1" ht="18.75">
-      <c r="A49" s="3">
+    <row r="49" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A49" s="24">
         <v>104010018</v>
       </c>
       <c r="B49" s="2" t="s">
         <v>49</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="50" customHeight="1" ht="18.75">
-      <c r="A50" s="3">
+    <row r="50" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A50" s="24">
         <v>104010019</v>
       </c>
       <c r="B50" s="2" t="s">
         <v>50</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="51" customHeight="1" ht="18.75">
-      <c r="A51" s="3">
+    <row r="51" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A51" s="24">
         <v>104010020</v>
       </c>
       <c r="B51" s="2" t="s">
         <v>51</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="52" customHeight="1" ht="18.75">
-      <c r="A52" s="3">
+    <row r="52" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A52" s="24">
         <v>104020001</v>
       </c>
       <c r="B52" s="2" t="s">
         <v>52</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="53" customHeight="1" ht="18.75">
-      <c r="A53" s="3">
+    <row r="53" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A53" s="24">
         <v>104030001</v>
       </c>
       <c r="B53" s="2" t="s">
         <v>53</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="54" customHeight="1" ht="18.75">
-      <c r="A54" s="3">
+    <row r="54" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A54" s="24">
         <v>104070001</v>
       </c>
       <c r="B54" s="2" t="s">
         <v>54</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="55" customHeight="1" ht="18.75">
-      <c r="A55" s="3">
+    <row r="55" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A55" s="24">
         <v>104070002</v>
       </c>
       <c r="B55" s="2" t="s">
         <v>55</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="56" customHeight="1" ht="18.75">
-      <c r="A56" s="3">
+    <row r="56" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A56" s="24">
         <v>104070003</v>
       </c>
       <c r="B56" s="2" t="s">
         <v>56</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="57" customHeight="1" ht="18.75">
-      <c r="A57" s="3">
+    <row r="57" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A57" s="24">
         <v>104070004</v>
       </c>
       <c r="B57" s="2" t="s">
         <v>57</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="58" customHeight="1" ht="18.75">
-      <c r="A58" s="3">
+    <row r="58" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A58" s="24">
         <v>104080001</v>
       </c>
       <c r="B58" s="2" t="s">
         <v>58</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="59" customHeight="1" ht="18.75">
-      <c r="A59" s="3">
+    <row r="59" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A59" s="24">
         <v>104110002</v>
       </c>
       <c r="B59" s="2" t="s">
         <v>59</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="60" customHeight="1" ht="18.75">
-      <c r="A60" s="3">
+    <row r="60" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A60" s="24">
         <v>104114100</v>
       </c>
       <c r="B60" s="2" t="s">
         <v>60</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="61" customHeight="1" ht="18.75">
-      <c r="A61" s="3">
+    <row r="61" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A61" s="24">
         <v>181030003</v>
       </c>
       <c r="B61" s="2" t="s">
         <v>61</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="62" customHeight="1" ht="18.75">
-      <c r="A62" s="3">
+    <row r="62" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A62" s="24">
         <v>181039901</v>
       </c>
       <c r="B62" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="63" customHeight="1" ht="18.75">
-      <c r="A63" s="3">
+    <row r="63" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A63" s="24">
         <v>181050009</v>
       </c>
       <c r="B63" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="64" customHeight="1" ht="18.75">
-      <c r="A64" s="3">
+    <row r="64" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A64" s="24">
         <v>181050010</v>
       </c>
       <c r="B64" s="2" t="s">
         <v>64</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="65" customHeight="1" ht="18.75">
-      <c r="A65" s="3">
+    <row r="65" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A65" s="24">
         <v>181050011</v>
       </c>
       <c r="B65" s="2" t="s">
         <v>65</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="66" customHeight="1" ht="18.75">
-      <c r="A66" s="3">
+    <row r="66" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A66" s="24">
         <v>181060003</v>
       </c>
       <c r="B66" s="2" t="s">
         <v>66</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="67" customHeight="1" ht="18.75">
-      <c r="A67" s="3">
+    <row r="67" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A67" s="24">
         <v>191010101</v>
       </c>
       <c r="B67" s="2" t="s">
         <v>67</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="68" customHeight="1" ht="18.75">
-      <c r="A68" s="3">
+    <row r="68" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A68" s="24">
         <v>191010102</v>
       </c>
       <c r="B68" s="2" t="s">
         <v>68</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="69" customHeight="1" ht="18.75">
-      <c r="A69" s="3">
+    <row r="69" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A69" s="24">
         <v>191010103</v>
       </c>
       <c r="B69" s="2" t="s">
         <v>69</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="70" customHeight="1" ht="18.75">
-      <c r="A70" s="3">
+    <row r="70" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A70" s="24">
         <v>192020205</v>
       </c>
       <c r="B70" s="2" t="s">
         <v>70</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="71" customHeight="1" ht="18.75">
-      <c r="A71" s="3">
+    <row r="71" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A71" s="24">
         <v>201010002</v>
       </c>
       <c r="B71" s="2" t="s">
         <v>71</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="72" customHeight="1" ht="18.75">
-      <c r="A72" s="3">
+    <row r="72" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A72" s="24">
         <v>201020002</v>
       </c>
       <c r="B72" s="2" t="s">
         <v>72</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="73" customHeight="1" ht="18.75">
-      <c r="A73" s="3">
+    <row r="73" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A73" s="24">
         <v>201040011</v>
       </c>
       <c r="B73" s="2" t="s">
         <v>73</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="74" customHeight="1" ht="18.75">
-      <c r="A74" s="3">
+    <row r="74" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A74" s="24">
         <v>201040012</v>
       </c>
       <c r="B74" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="75" customHeight="1" ht="18.75">
-      <c r="A75" s="3">
+    <row r="75" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A75" s="24">
         <v>201040013</v>
       </c>
       <c r="B75" s="2" t="s">
         <v>75</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="76" customHeight="1" ht="18.75">
-      <c r="A76" s="3">
+    <row r="76" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A76" s="24">
         <v>201040014</v>
       </c>
       <c r="B76" s="2" t="s">
         <v>76</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="77" customHeight="1" ht="18.75">
-      <c r="A77" s="3">
+    <row r="77" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A77" s="24">
         <v>201040016</v>
       </c>
       <c r="B77" s="2" t="s">
         <v>77</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="78" customHeight="1" ht="18.75">
-      <c r="A78" s="3">
+    <row r="78" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A78" s="24">
         <v>201040017</v>
       </c>
       <c r="B78" s="2" t="s">
         <v>78</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="79" customHeight="1" ht="18.75">
-      <c r="A79" s="3">
+    <row r="79" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A79" s="24">
         <v>201040018</v>
       </c>
       <c r="B79" s="2" t="s">
         <v>79</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="80" customHeight="1" ht="18.75">
-      <c r="A80" s="3">
+    <row r="80" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A80" s="24">
         <v>201040019</v>
       </c>
       <c r="B80" s="2" t="s">
         <v>80</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="81" customHeight="1" ht="18.75">
-      <c r="A81" s="3">
+    <row r="81" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A81" s="24">
         <v>201040020</v>
       </c>
       <c r="B81" s="2" t="s">
         <v>81</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="82" customHeight="1" ht="18.75">
-      <c r="A82" s="3">
+    <row r="82" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A82" s="24">
         <v>202030004</v>
       </c>
       <c r="B82" s="2" t="s">
         <v>82</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="83" customHeight="1" ht="18.75">
-      <c r="A83" s="3">
+    <row r="83" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A83" s="24">
         <v>202050006</v>
       </c>
       <c r="B83" s="2" t="s">
         <v>83</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="84" customHeight="1" ht="18.75">
-      <c r="A84" s="3">
+    <row r="84" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A84" s="24">
         <v>203030007</v>
       </c>
       <c r="B84" s="2" t="s">
         <v>84</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="85" customHeight="1" ht="18.75">
-      <c r="A85" s="3">
+    <row r="85" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A85" s="24">
         <v>204020004</v>
       </c>
       <c r="B85" s="2" t="s">
         <v>85</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="86" customHeight="1" ht="18.75">
-      <c r="A86" s="3">
+    <row r="86" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A86" s="24">
         <v>204020005</v>
       </c>
       <c r="B86" s="2" t="s">
         <v>86</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="87" customHeight="1" ht="18.75">
-      <c r="A87" s="3">
+    <row r="87" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A87" s="24">
         <v>204020006</v>
       </c>
       <c r="B87" s="2" t="s">
         <v>87</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="88" customHeight="1" ht="18.75">
-      <c r="A88" s="3">
+    <row r="88" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A88" s="24">
         <v>204020007</v>
       </c>
       <c r="B88" s="2" t="s">
         <v>88</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="89" customHeight="1" ht="18.75">
-      <c r="A89" s="3">
+    <row r="89" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A89" s="24">
         <v>204020009</v>
       </c>
       <c r="B89" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="90" customHeight="1" ht="18.75">
-      <c r="A90" s="3">
+    <row r="90" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A90" s="24">
         <v>204020010</v>
       </c>
       <c r="B90" s="2" t="s">
         <v>90</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="91" customHeight="1" ht="18.75">
-      <c r="A91" s="3">
+    <row r="91" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A91" s="24">
         <v>204020011</v>
       </c>
       <c r="B91" s="2" t="s">
         <v>91</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="92" customHeight="1" ht="18.75">
-      <c r="A92" s="3">
+    <row r="92" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A92" s="24">
         <v>204020012</v>
       </c>
       <c r="B92" s="2" t="s">
         <v>92</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="93" customHeight="1" ht="18.75">
-      <c r="A93" s="3">
+    <row r="93" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A93" s="24">
         <v>204030002</v>
       </c>
       <c r="B93" s="2" t="s">
         <v>93</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="94" customHeight="1" ht="18.75">
-      <c r="A94" s="3">
+    <row r="94" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A94" s="24">
         <v>204030003</v>
       </c>
       <c r="B94" s="2" t="s">
         <v>94</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="95" customHeight="1" ht="18.75">
-      <c r="A95" s="3">
+    <row r="95" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A95" s="24">
         <v>204030006</v>
       </c>
       <c r="B95" s="2" t="s">
         <v>95</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="96" customHeight="1" ht="18.75">
-      <c r="A96" s="3">
+    <row r="96" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A96" s="24">
         <v>204030008</v>
       </c>
       <c r="B96" s="2" t="s">
         <v>96</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="97" customHeight="1" ht="18.75">
-      <c r="A97" s="3">
+    <row r="97" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A97" s="24">
         <v>204030015</v>
       </c>
       <c r="B97" s="2" t="s">
         <v>97</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="98" customHeight="1" ht="18.75">
-      <c r="A98" s="3">
+    <row r="98" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A98" s="24">
         <v>204030018</v>
       </c>
       <c r="B98" s="2" t="s">
         <v>98</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="99" customHeight="1" ht="18.75">
-      <c r="A99" s="3">
+    <row r="99" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A99" s="24">
         <v>204040001</v>
       </c>
       <c r="B99" s="2" t="s">
         <v>99</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="100" customHeight="1" ht="18.75">
-      <c r="A100" s="3">
+    <row r="100" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A100" s="24">
         <v>204040003</v>
       </c>
       <c r="B100" s="2" t="s">
         <v>100</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="101" customHeight="1" ht="18.75">
-      <c r="A101" s="3">
+    <row r="101" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A101" s="24">
         <v>204050001</v>
       </c>
       <c r="B101" s="2" t="s">
         <v>101</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="102" customHeight="1" ht="18.75">
-      <c r="A102" s="3">
+    <row r="102" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A102" s="24">
         <v>204050002</v>
       </c>
       <c r="B102" s="2" t="s">
         <v>102</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="103" customHeight="1" ht="18.75">
-      <c r="A103" s="3">
+    <row r="103" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A103" s="24">
         <v>204050003</v>
       </c>
       <c r="B103" s="2" t="s">
         <v>103</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="104" customHeight="1" ht="18.75">
-      <c r="A104" s="3">
+    <row r="104" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A104" s="24">
         <v>204050004</v>
       </c>
       <c r="B104" s="2" t="s">
         <v>104</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="105" customHeight="1" ht="18.75">
-      <c r="A105" s="3">
+    <row r="105" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A105" s="24">
         <v>204080001</v>
       </c>
       <c r="B105" s="2" t="s">
         <v>105</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="106" customHeight="1" ht="18.75">
-      <c r="A106" s="3">
+    <row r="106" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A106" s="24">
         <v>204080002</v>
       </c>
       <c r="B106" s="2" t="s">
         <v>106</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="107" customHeight="1" ht="18.75">
-      <c r="A107" s="3">
+    <row r="107" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A107" s="24">
         <v>205020002</v>
       </c>
       <c r="B107" s="2" t="s">
         <v>107</v>
       </c>
     </row>
-    <row x14ac:dyDescent="0.25" r="108" customHeight="1" ht="18.75">
-      <c r="A108" s="3">
+    <row r="108" spans="1:2" ht="18.75" customHeight="1">
+      <c r="A108" s="24">
         <v>205060002</v>
       </c>
       <c r="B108" s="2" t="s">

</xml_diff>

<commit_message>
update program and condition
</commit_message>
<xml_diff>
--- a/Program/condition.xlsx
+++ b/Program/condition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_filtering\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53EB623C-FC10-4623-9A30-FA7484880527}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548CC5C0-6C4E-4E0B-B23C-64F7DC124837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1083,27 +1083,9 @@
     <t>51XXXXXX</t>
   </si>
   <si>
-    <t>รหัสกิจกรรม N0301</t>
-  </si>
-  <si>
-    <t>N0301$</t>
-  </si>
-  <si>
     <t>54XXXXXX</t>
   </si>
   <si>
-    <t>รหัสกิจกรรม N0104</t>
-  </si>
-  <si>
-    <t>N0104$</t>
-  </si>
-  <si>
-    <t>รหัสกิจกรรม N0105</t>
-  </si>
-  <si>
-    <t>N0105$</t>
-  </si>
-  <si>
     <t>59XXXXXX</t>
   </si>
   <si>
@@ -1210,6 +1192,24 @@
   </si>
   <si>
     <t>^(?!.*[EN].{0,4}$)</t>
+  </si>
+  <si>
+    <t>act N0104</t>
+  </si>
+  <si>
+    <t>act N0301</t>
+  </si>
+  <si>
+    <t>act N0105</t>
+  </si>
+  <si>
+    <t>รหัสกิจกรรม N0301 รหัสบัญชี 51XXXXXX เท่านั้น</t>
+  </si>
+  <si>
+    <t>รหัสกิจกรรม N0104 รหัสบัญชี 54XXXXXX เท่านั้น</t>
+  </si>
+  <si>
+    <t>รหัสกิจกรรม N0105 รหัสบัญชี 54XXXXXX เท่านั้น</t>
   </si>
 </sst>
 </file>
@@ -1664,7 +1664,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15" t="s">
-        <v>391</v>
+        <v>385</v>
       </c>
       <c r="F2" s="15"/>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="F3" s="15"/>
     </row>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15" t="s">
-        <v>393</v>
+        <v>387</v>
       </c>
       <c r="F4" s="15"/>
     </row>
@@ -1811,64 +1811,64 @@
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>353</v>
+        <v>393</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15" t="s">
-        <v>354</v>
+        <v>391</v>
       </c>
       <c r="F9" s="15"/>
     </row>
     <row r="10" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A10" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
-        <v>356</v>
+        <v>394</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15" t="s">
-        <v>357</v>
+        <v>390</v>
       </c>
       <c r="F10" s="15"/>
     </row>
     <row r="11" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A11" s="13" t="s">
-        <v>355</v>
+        <v>353</v>
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14" t="s">
-        <v>358</v>
+        <v>395</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15" t="s">
-        <v>359</v>
+        <v>392</v>
       </c>
       <c r="F11" s="15"/>
     </row>
     <row r="12" spans="1:6" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A12" s="17" t="s">
-        <v>360</v>
+        <v>354</v>
       </c>
       <c r="B12" s="18" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>362</v>
+        <v>356</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>363</v>
+        <v>357</v>
       </c>
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>364</v>
+        <v>358</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>365</v>
+        <v>359</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>343</v>
@@ -1879,38 +1879,38 @@
     </row>
     <row r="14" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A14" s="13" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14" t="s">
-        <v>367</v>
+        <v>361</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15" t="s">
-        <v>390</v>
+        <v>384</v>
       </c>
       <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A15" s="13" t="s">
-        <v>366</v>
+        <v>360</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14" t="s">
-        <v>368</v>
+        <v>362</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15" t="s">
-        <v>392</v>
+        <v>386</v>
       </c>
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>369</v>
+        <v>363</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>370</v>
+        <v>364</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>343</v>
@@ -1921,10 +1921,10 @@
     </row>
     <row r="17" spans="1:6" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>371</v>
+        <v>365</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>372</v>
+        <v>366</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>343</v>
@@ -1935,10 +1935,10 @@
     </row>
     <row r="18" spans="1:6" s="12" customFormat="1" ht="20.25" customHeight="1">
       <c r="A18" s="17" t="s">
-        <v>373</v>
+        <v>367</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>374</v>
+        <v>368</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>343</v>
@@ -1949,10 +1949,10 @@
     </row>
     <row r="19" spans="1:6" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A19" s="17" t="s">
-        <v>375</v>
+        <v>369</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>376</v>
+        <v>370</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>343</v>
@@ -1963,10 +1963,10 @@
     </row>
     <row r="20" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>377</v>
+        <v>371</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>378</v>
+        <v>372</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>343</v>
@@ -1977,65 +1977,65 @@
     </row>
     <row r="21" spans="1:6" s="12" customFormat="1" ht="20.25" customHeight="1">
       <c r="A21" s="17" t="s">
-        <v>379</v>
+        <v>373</v>
       </c>
       <c r="B21" s="18" t="s">
-        <v>380</v>
+        <v>374</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>381</v>
+        <v>375</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14" t="s">
-        <v>395</v>
+        <v>389</v>
       </c>
       <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" s="12" customFormat="1" ht="20.25" customHeight="1">
       <c r="A22" s="17" t="s">
-        <v>382</v>
+        <v>376</v>
       </c>
       <c r="B22" s="18" t="s">
-        <v>383</v>
+        <v>377</v>
       </c>
       <c r="C22" s="14" t="s">
-        <v>384</v>
+        <v>378</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14" t="s">
-        <v>394</v>
+        <v>388</v>
       </c>
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1">
       <c r="A23" s="17" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B23" s="18" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>386</v>
+        <v>380</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="9" t="s">
-        <v>387</v>
+        <v>381</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A24" s="17" t="s">
-        <v>385</v>
+        <v>379</v>
       </c>
       <c r="B24" s="18" t="s">
-        <v>361</v>
+        <v>355</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>388</v>
+        <v>382</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14" t="s">
-        <v>389</v>
+        <v>383</v>
       </c>
       <c r="F24" s="14"/>
     </row>

</xml_diff>

<commit_message>
add condition 2 column in result
</commit_message>
<xml_diff>
--- a/Program/condition.xlsx
+++ b/Program/condition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_filtering\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{548CC5C0-6C4E-4E0B-B23C-64F7DC124837}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FF1142-920F-4A32-865A-725871AF4FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1664,7 +1664,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>

<commit_message>
change product to segment
</commit_message>
<xml_diff>
--- a/Program/condition.xlsx
+++ b/Program/condition.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\database_filtering\Program\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A1FF1142-920F-4A32-865A-725871AF4FE4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{01792AA2-A1AF-4CE6-B7F3-8DCEF2624DB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1092,12 +1092,6 @@
     <t>ค่าใช้จ่าย</t>
   </si>
   <si>
-    <t>บันทึกเข้า Product 192020001</t>
-  </si>
-  <si>
-    <t>product 192020001</t>
-  </si>
-  <si>
     <t>5X641XXX</t>
   </si>
   <si>
@@ -1210,6 +1204,12 @@
   </si>
   <si>
     <t>รหัสกิจกรรม N0105 รหัสบัญชี 54XXXXXX เท่านั้น</t>
+  </si>
+  <si>
+    <t>segment 19202</t>
+  </si>
+  <si>
+    <t>บันทึกเข้า เซกเมนต์ 19202</t>
   </si>
 </sst>
 </file>
@@ -1664,7 +1664,7 @@
   <dimension ref="A1:F24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="F12" sqref="F12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -1709,7 +1709,7 @@
       </c>
       <c r="D2" s="15"/>
       <c r="E2" s="15" t="s">
-        <v>385</v>
+        <v>383</v>
       </c>
       <c r="F2" s="15"/>
     </row>
@@ -1725,7 +1725,7 @@
       </c>
       <c r="D3" s="15"/>
       <c r="E3" s="15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F3" s="15"/>
     </row>
@@ -1741,7 +1741,7 @@
       </c>
       <c r="D4" s="15"/>
       <c r="E4" s="15" t="s">
-        <v>387</v>
+        <v>385</v>
       </c>
       <c r="F4" s="15"/>
     </row>
@@ -1811,11 +1811,11 @@
       </c>
       <c r="B9" s="14"/>
       <c r="C9" s="14" t="s">
-        <v>393</v>
+        <v>391</v>
       </c>
       <c r="D9" s="15"/>
       <c r="E9" s="15" t="s">
-        <v>391</v>
+        <v>389</v>
       </c>
       <c r="F9" s="15"/>
     </row>
@@ -1825,11 +1825,11 @@
       </c>
       <c r="B10" s="14"/>
       <c r="C10" s="14" t="s">
-        <v>394</v>
+        <v>392</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="15" t="s">
-        <v>390</v>
+        <v>388</v>
       </c>
       <c r="F10" s="15"/>
     </row>
@@ -1839,15 +1839,15 @@
       </c>
       <c r="B11" s="14"/>
       <c r="C11" s="14" t="s">
-        <v>395</v>
+        <v>393</v>
       </c>
       <c r="D11" s="15"/>
       <c r="E11" s="15" t="s">
-        <v>392</v>
+        <v>390</v>
       </c>
       <c r="F11" s="15"/>
     </row>
-    <row r="12" spans="1:6" s="12" customFormat="1" ht="21" customHeight="1">
+    <row r="12" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A12" s="17" t="s">
         <v>354</v>
       </c>
@@ -1855,20 +1855,20 @@
         <v>355</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>356</v>
+        <v>395</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14" t="s">
-        <v>357</v>
+        <v>394</v>
       </c>
       <c r="F12" s="14"/>
     </row>
     <row r="13" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A13" s="13" t="s">
-        <v>358</v>
+        <v>356</v>
       </c>
       <c r="B13" s="14" t="s">
-        <v>359</v>
+        <v>357</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>343</v>
@@ -1879,38 +1879,38 @@
     </row>
     <row r="14" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A14" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B14" s="14"/>
       <c r="C14" s="14" t="s">
-        <v>361</v>
+        <v>359</v>
       </c>
       <c r="D14" s="15"/>
       <c r="E14" s="15" t="s">
-        <v>384</v>
+        <v>382</v>
       </c>
       <c r="F14" s="15"/>
     </row>
     <row r="15" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A15" s="13" t="s">
-        <v>360</v>
+        <v>358</v>
       </c>
       <c r="B15" s="14"/>
       <c r="C15" s="14" t="s">
-        <v>362</v>
+        <v>360</v>
       </c>
       <c r="D15" s="15"/>
       <c r="E15" s="15" t="s">
-        <v>386</v>
+        <v>384</v>
       </c>
       <c r="F15" s="15"/>
     </row>
     <row r="16" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A16" s="13" t="s">
-        <v>363</v>
+        <v>361</v>
       </c>
       <c r="B16" s="14" t="s">
-        <v>364</v>
+        <v>362</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>343</v>
@@ -1921,10 +1921,10 @@
     </row>
     <row r="17" spans="1:6" s="12" customFormat="1" ht="19.5" customHeight="1">
       <c r="A17" s="17" t="s">
-        <v>365</v>
+        <v>363</v>
       </c>
       <c r="B17" s="14" t="s">
-        <v>366</v>
+        <v>364</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>343</v>
@@ -1935,10 +1935,10 @@
     </row>
     <row r="18" spans="1:6" s="12" customFormat="1" ht="20.25" customHeight="1">
       <c r="A18" s="17" t="s">
-        <v>367</v>
+        <v>365</v>
       </c>
       <c r="B18" s="18" t="s">
-        <v>368</v>
+        <v>366</v>
       </c>
       <c r="C18" s="14" t="s">
         <v>343</v>
@@ -1949,10 +1949,10 @@
     </row>
     <row r="19" spans="1:6" s="12" customFormat="1" ht="21" customHeight="1">
       <c r="A19" s="17" t="s">
-        <v>369</v>
+        <v>367</v>
       </c>
       <c r="B19" s="18" t="s">
-        <v>370</v>
+        <v>368</v>
       </c>
       <c r="C19" s="14" t="s">
         <v>343</v>
@@ -1963,10 +1963,10 @@
     </row>
     <row r="20" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A20" s="19" t="s">
-        <v>371</v>
+        <v>369</v>
       </c>
       <c r="B20" s="14" t="s">
-        <v>372</v>
+        <v>370</v>
       </c>
       <c r="C20" s="14" t="s">
         <v>343</v>
@@ -1977,65 +1977,65 @@
     </row>
     <row r="21" spans="1:6" s="12" customFormat="1" ht="20.25" customHeight="1">
       <c r="A21" s="17" t="s">
+        <v>371</v>
+      </c>
+      <c r="B21" s="18" t="s">
+        <v>372</v>
+      </c>
+      <c r="C21" s="14" t="s">
         <v>373</v>
-      </c>
-      <c r="B21" s="18" t="s">
-        <v>374</v>
-      </c>
-      <c r="C21" s="14" t="s">
-        <v>375</v>
       </c>
       <c r="D21" s="14"/>
       <c r="E21" s="14" t="s">
-        <v>389</v>
+        <v>387</v>
       </c>
       <c r="F21" s="14"/>
     </row>
     <row r="22" spans="1:6" s="12" customFormat="1" ht="20.25" customHeight="1">
       <c r="A22" s="17" t="s">
+        <v>374</v>
+      </c>
+      <c r="B22" s="18" t="s">
+        <v>375</v>
+      </c>
+      <c r="C22" s="14" t="s">
         <v>376</v>
-      </c>
-      <c r="B22" s="18" t="s">
-        <v>377</v>
-      </c>
-      <c r="C22" s="14" t="s">
-        <v>378</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14" t="s">
-        <v>388</v>
+        <v>386</v>
       </c>
       <c r="F22" s="14"/>
     </row>
     <row r="23" spans="1:6" ht="18.75" customHeight="1">
       <c r="A23" s="17" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B23" s="18" t="s">
         <v>355</v>
       </c>
       <c r="C23" s="20" t="s">
-        <v>380</v>
+        <v>378</v>
       </c>
       <c r="D23" s="15"/>
       <c r="E23" s="9" t="s">
-        <v>381</v>
+        <v>379</v>
       </c>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" s="12" customFormat="1" ht="18.75" customHeight="1">
       <c r="A24" s="17" t="s">
-        <v>379</v>
+        <v>377</v>
       </c>
       <c r="B24" s="18" t="s">
         <v>355</v>
       </c>
       <c r="C24" s="20" t="s">
-        <v>382</v>
+        <v>380</v>
       </c>
       <c r="D24" s="14"/>
       <c r="E24" s="14" t="s">
-        <v>383</v>
+        <v>381</v>
       </c>
       <c r="F24" s="14"/>
     </row>

</xml_diff>